<commit_message>
correction purchased seed fp + draft lhc
</commit_message>
<xml_diff>
--- a/data/comp_var_Paul_thesis_vs_TAMASA.xlsx
+++ b/data/comp_var_Paul_thesis_vs_TAMASA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\TAMASA\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{80F2A1AF-11F4-40FF-9468-D344169F110D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DA692F63-86B1-4BA9-AB50-E467870CF4E1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="7875" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18195" windowHeight="7875" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="costs_local_currency" sheetId="1" r:id="rId1"/>
@@ -424,7 +424,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="96">
   <si>
     <t>Country</t>
   </si>
@@ -709,6 +709,9 @@
   </si>
   <si>
     <t>can be calculated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no data </t>
   </si>
 </sst>
 </file>
@@ -4974,8 +4977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D06573A-A8F5-4AAD-B0B3-6E8108579E0D}">
   <dimension ref="A1:D16380"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5126,7 +5129,7 @@
         <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -54296,7 +54299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC075E56-F992-4327-8882-486F052FBF46}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -54427,6 +54430,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009810AB5F2911E64683BAEC42E7B886E6" ma:contentTypeVersion="8" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="ca1fbb159048343a84ed76b6e4d91d8d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="42935c7d-9f47-4399-b135-59bc620e0da9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d462d4cd21746c9dd51fafdfa118bae1" ns3:_="">
     <xsd:import namespace="42935c7d-9f47-4399-b135-59bc620e0da9"/>
@@ -54596,22 +54614,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BFD4D3D-3296-4263-B14C-5DD7535BCB14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="42935c7d-9f47-4399-b135-59bc620e0da9"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E711286-A16B-44D6-85BE-61591783C649}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B921580B-FE11-49B1-BAD4-9EA660F15EBD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54627,28 +54654,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E711286-A16B-44D6-85BE-61591783C649}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BFD4D3D-3296-4263-B14C-5DD7535BCB14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="42935c7d-9f47-4399-b135-59bc620e0da9"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>